<commit_message>
Corrida - proyecto simulacion-web
</commit_message>
<xml_diff>
--- a/tablas/04_Rollos_Apilamiento_Resultado_Completo.xlsx
+++ b/tablas/04_Rollos_Apilamiento_Resultado_Completo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AB6"/>
+  <dimension ref="A1:AB5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -859,7 +859,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>663</v>
+        <v>474</v>
       </c>
       <c r="B5" t="n">
         <v>1</v>
@@ -868,34 +868,34 @@
         <v>0.8</v>
       </c>
       <c r="D5" t="n">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E5" t="n">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="F5" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="G5" t="n">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="H5" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>14.4</v>
+        <v>11.2</v>
       </c>
       <c r="L5" t="n">
-        <v>14.2</v>
+        <v>13.1</v>
       </c>
       <c r="M5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="N5" t="n">
         <v>0</v>
@@ -904,16 +904,16 @@
         <v>0</v>
       </c>
       <c r="P5" t="n">
-        <v>0</v>
+        <v>4.800000000000001</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>1.1</v>
       </c>
       <c r="R5" t="n">
-        <v>204.48</v>
+        <v>146.72</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>5.280000000000001</v>
       </c>
       <c r="T5" t="n">
         <v>13</v>
@@ -923,7 +923,7 @@
       </c>
       <c r="V5" t="inlineStr">
         <is>
-          <t>Ajuste por base</t>
+          <t>Normal</t>
         </is>
       </c>
       <c r="W5" t="inlineStr">
@@ -937,7 +937,7 @@
         </is>
       </c>
       <c r="Y5" t="n">
-        <v>663</v>
+        <v>474</v>
       </c>
       <c r="Z5" t="n">
         <v>0</v>
@@ -946,100 +946,6 @@
         <v>25</v>
       </c>
       <c r="AB5" t="inlineStr">
-        <is>
-          <t>arriba</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>11</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D6" t="n">
-        <v>4</v>
-      </c>
-      <c r="E6" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" t="n">
-        <v>9</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" t="n">
-        <v>2</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" t="n">
-        <v>2</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0</v>
-      </c>
-      <c r="P6" t="n">
-        <v>1.6</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>1.1</v>
-      </c>
-      <c r="R6" t="n">
-        <v>3.2</v>
-      </c>
-      <c r="S6" t="n">
-        <v>1.76</v>
-      </c>
-      <c r="T6" t="n">
-        <v>2</v>
-      </c>
-      <c r="U6" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="V6" t="inlineStr">
-        <is>
-          <t>Normal</t>
-        </is>
-      </c>
-      <c r="W6" t="inlineStr">
-        <is>
-          <t>MTR02</t>
-        </is>
-      </c>
-      <c r="X6" t="inlineStr">
-        <is>
-          <t>20x15</t>
-        </is>
-      </c>
-      <c r="Y6" t="n">
-        <v>11</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>20</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>25</v>
-      </c>
-      <c r="AB6" t="inlineStr">
         <is>
           <t>arriba</t>
         </is>

</xml_diff>